<commit_message>
Fixed some responsivity issues and some translations
</commit_message>
<xml_diff>
--- a/static/data/public/data.xlsx
+++ b/static/data/public/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,12 +512,6 @@
     <t>sukkar</t>
   </si>
   <si>
-    <t>burtuqaal</t>
-  </si>
-  <si>
-    <t>manga</t>
-  </si>
-  <si>
     <t>بِرتُقال</t>
   </si>
   <si>
@@ -596,9 +590,6 @@
     <t>marraat</t>
   </si>
   <si>
-    <t>3aadatan</t>
-  </si>
-  <si>
     <t>ghaaliban</t>
   </si>
   <si>
@@ -1008,6 +999,15 @@
   </si>
   <si>
     <t>غَرب</t>
+  </si>
+  <si>
+    <t>manja</t>
+  </si>
+  <si>
+    <t>3aadan</t>
+  </si>
+  <si>
+    <t>bertuqaal</t>
   </si>
 </sst>
 </file>
@@ -1372,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="116" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.35"/>
@@ -1407,16 +1407,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1424,16 +1424,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1441,16 +1441,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1458,16 +1458,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1475,16 +1475,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1492,16 +1492,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1509,16 +1509,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1526,16 +1526,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1543,16 +1543,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1560,16 +1560,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1577,16 +1577,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1594,16 +1594,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1611,16 +1611,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1628,16 +1628,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1645,16 +1645,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1662,16 +1662,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1679,16 +1679,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1696,16 +1696,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1713,16 +1713,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1730,16 +1730,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1747,16 +1747,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1764,16 +1764,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1781,16 +1781,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1798,16 +1798,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1815,16 +1815,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1849,13 +1849,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
@@ -1934,13 +1934,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>7</v>
@@ -2002,13 +2002,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>7</v>
@@ -2019,13 +2019,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>7</v>
@@ -2104,13 +2104,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
@@ -2121,13 +2121,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>7</v>
@@ -2138,13 +2138,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>7</v>
@@ -2155,13 +2155,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>7</v>
@@ -2172,7 +2172,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>13</v>
@@ -2189,13 +2189,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>7</v>
@@ -2291,13 +2291,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>189</v>
+        <v>325</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>7</v>
@@ -2427,16 +2427,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2444,16 +2444,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2461,16 +2461,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2478,16 +2478,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2495,16 +2495,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2512,16 +2512,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2529,16 +2529,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2546,16 +2546,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2563,16 +2563,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2580,16 +2580,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2597,16 +2597,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2614,16 +2614,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2631,16 +2631,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2648,16 +2648,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2665,16 +2665,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2682,7 +2682,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>140</v>
@@ -2818,7 +2818,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>26</v>
@@ -2835,7 +2835,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>142</v>
@@ -2886,7 +2886,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>139</v>
@@ -2903,7 +2903,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>145</v>
@@ -2920,13 +2920,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>162</v>
+        <v>324</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>40</v>
@@ -2971,7 +2971,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>150</v>
@@ -3022,13 +3022,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>161</v>
+        <v>326</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>40</v>
@@ -3056,7 +3056,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>149</v>
@@ -3073,7 +3073,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>143</v>
@@ -3107,7 +3107,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>159</v>
@@ -3141,7 +3141,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>151</v>
@@ -3158,7 +3158,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Small corrections and additions
</commit_message>
<xml_diff>
--- a/static/data/public/data.xlsx
+++ b/static/data/public/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="333">
   <si>
     <t>arabic</t>
   </si>
@@ -512,9 +512,6 @@
     <t>sukkar</t>
   </si>
   <si>
-    <t>بِرتُقال</t>
-  </si>
-  <si>
     <t>ليمون</t>
   </si>
   <si>
@@ -833,9 +830,6 @@
     <t>lameen</t>
   </si>
   <si>
-    <t>mata</t>
-  </si>
-  <si>
     <t>شو</t>
   </si>
   <si>
@@ -1007,7 +1001,31 @@
     <t>3aadan</t>
   </si>
   <si>
-    <t>bertuqaal</t>
+    <t>بُرتُقال</t>
+  </si>
+  <si>
+    <t>burtuqaal</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>مِلِح</t>
+  </si>
+  <si>
+    <t>meleh</t>
+  </si>
+  <si>
+    <t>فِلفِل</t>
+  </si>
+  <si>
+    <t>filfil</t>
+  </si>
+  <si>
+    <t>mataa</t>
   </si>
 </sst>
 </file>
@@ -1370,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="116" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.35"/>
@@ -1407,16 +1425,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1424,16 +1442,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1441,16 +1459,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1458,16 +1476,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1475,16 +1493,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1492,16 +1510,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1509,16 +1527,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1526,16 +1544,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1543,16 +1561,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1560,16 +1578,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1577,16 +1595,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1594,16 +1612,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1611,16 +1629,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1628,16 +1646,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1645,16 +1663,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1662,16 +1680,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1679,16 +1697,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1696,16 +1714,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1713,16 +1731,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1730,16 +1748,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1747,16 +1765,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1764,16 +1782,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1781,16 +1799,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1798,16 +1816,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1815,16 +1833,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1849,13 +1867,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
@@ -1934,13 +1952,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>7</v>
@@ -2002,13 +2020,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>7</v>
@@ -2019,13 +2037,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>7</v>
@@ -2104,13 +2122,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
@@ -2121,13 +2139,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>7</v>
@@ -2138,13 +2156,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>7</v>
@@ -2155,13 +2173,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>7</v>
@@ -2172,7 +2190,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>13</v>
@@ -2189,13 +2207,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>7</v>
@@ -2291,13 +2309,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>7</v>
@@ -2427,16 +2445,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2444,16 +2462,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2461,16 +2479,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2478,16 +2496,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2495,16 +2513,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2512,16 +2530,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2529,16 +2547,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2546,16 +2564,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2563,16 +2581,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2580,16 +2598,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2597,16 +2615,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2614,16 +2632,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2631,16 +2649,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2648,16 +2666,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2665,16 +2683,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2682,7 +2700,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>140</v>
@@ -2818,7 +2836,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>26</v>
@@ -2835,7 +2853,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>142</v>
@@ -2886,7 +2904,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>139</v>
@@ -2903,7 +2921,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>145</v>
@@ -2920,13 +2938,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>40</v>
@@ -2971,7 +2989,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>150</v>
@@ -3022,13 +3040,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>161</v>
+        <v>324</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>40</v>
@@ -3056,7 +3074,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>149</v>
@@ -3073,7 +3091,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>143</v>
@@ -3107,7 +3125,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>159</v>
@@ -3141,7 +3159,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>151</v>
@@ -3158,7 +3176,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>144</v>
@@ -3203,6 +3221,68 @@
       <c r="E107" s="1" t="s">
         <v>40</v>
       </c>
+    </row>
+    <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>107</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>108</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B110" s="7"/>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111" s="7"/>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B112" s="7"/>
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113" s="7"/>
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="7"/>
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="7"/>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116" s="7"/>
+      <c r="E116" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:E107">

</xml_diff>